<commit_message>
Added tile material to repo
</commit_message>
<xml_diff>
--- a/Tiles/Tiles.xlsx
+++ b/Tiles/Tiles.xlsx
@@ -2,17 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LiU\TSEA83\ZigSound\Tiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16305" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16305" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blunicorn" sheetId="1" r:id="rId1"/>
+    <sheet name="Tree 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,6 +22,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="3">
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>9B</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34,7 +49,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -44,6 +59,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFECC17"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF56CCF4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4EB2D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4075BB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -75,16 +114,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF4075BB"/>
+      <color rgb="FF400000"/>
+      <color rgb="FF4EB2D6"/>
+      <color rgb="FF56CCF4"/>
+      <color rgb="FFFECC17"/>
+      <color rgb="FFFBF237"/>
+      <color rgb="FFFFFA16"/>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -359,10 +414,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +442,9 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="P1" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -399,11 +457,15 @@
       <c r="H2" s="2"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="K2" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="O2" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -416,11 +478,19 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="M3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
@@ -433,6 +503,528 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
+      <c r="I4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5">
+        <v>97</v>
+      </c>
+      <c r="O6" s="5">
+        <v>97</v>
+      </c>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="5">
+        <v>97</v>
+      </c>
+      <c r="E16" s="5">
+        <v>97</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="5">
+        <v>97</v>
+      </c>
+      <c r="L16" s="5">
+        <v>97</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -443,14 +1035,14 @@
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -461,14 +1053,14 @@
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -479,14 +1071,14 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -497,14 +1089,14 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>

</xml_diff>